<commit_message>
import all products, cart model and routes
</commit_message>
<xml_diff>
--- a/server/ecommerce_data/ecommerce_data.xlsx
+++ b/server/ecommerce_data/ecommerce_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\OneDrive\Desktop\webdevstuff\Projects\ecommerce\server\ecommerce_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EC2057-9751-46E8-99D0-4D0ABAB3900F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1373268C-0743-4558-9770-7DACDC8EDB4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CDB3ECD7-B6AF-4BFD-B9A1-8F83DF4A6C4D}"/>
   </bookViews>
@@ -2430,9 +2430,6 @@
     <t>appellation</t>
   </si>
   <si>
-    <t>sub_style</t>
-  </si>
-  <si>
     <t>beers</t>
   </si>
   <si>
@@ -2440,6 +2437,9 @@
   </si>
   <si>
     <t>spirits</t>
+  </si>
+  <si>
+    <t>subtype</t>
   </si>
 </sst>
 </file>
@@ -3047,8 +3047,8 @@
   <dimension ref="A1:X139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:C1048576"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3109,7 +3109,7 @@
         <v>781</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>794</v>
+        <v>797</v>
       </c>
       <c r="L1" s="12" t="s">
         <v>782</v>
@@ -3150,7 +3150,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>2</v>
@@ -3210,7 +3210,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>2</v>
@@ -3270,7 +3270,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>12</v>
@@ -3328,7 +3328,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>12</v>
@@ -3386,7 +3386,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>18</v>
@@ -3444,7 +3444,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>18</v>
@@ -3502,7 +3502,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>26</v>
@@ -3560,7 +3560,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>26</v>
@@ -3618,7 +3618,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>30</v>
@@ -3676,7 +3676,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>30</v>
@@ -3734,7 +3734,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>37</v>
@@ -3792,7 +3792,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>37</v>
@@ -3850,7 +3850,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>46</v>
@@ -3908,7 +3908,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>46</v>
@@ -3966,7 +3966,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>53</v>
@@ -4024,7 +4024,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>53</v>
@@ -4082,7 +4082,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>61</v>
@@ -4140,7 +4140,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>61</v>
@@ -4198,7 +4198,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>69</v>
@@ -4252,7 +4252,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>73</v>
@@ -4306,7 +4306,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>76</v>
@@ -4360,7 +4360,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>79</v>
@@ -4414,7 +4414,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>88</v>
@@ -4468,7 +4468,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>93</v>
@@ -4522,7 +4522,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>96</v>
@@ -4576,7 +4576,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>100</v>
@@ -4634,7 +4634,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>100</v>
@@ -4692,7 +4692,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>107</v>
@@ -4750,7 +4750,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>110</v>
@@ -4808,7 +4808,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>110</v>
@@ -4866,7 +4866,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>119</v>
@@ -4924,7 +4924,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>119</v>
@@ -4982,7 +4982,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>127</v>
@@ -5040,7 +5040,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>127</v>
@@ -5098,7 +5098,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>133</v>
@@ -5156,7 +5156,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>133</v>
@@ -5214,7 +5214,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>144</v>
@@ -5272,7 +5272,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>144</v>
@@ -5330,7 +5330,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>148</v>
@@ -5388,7 +5388,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>190</v>
@@ -5448,7 +5448,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>196</v>
@@ -5504,7 +5504,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>201</v>
@@ -5562,7 +5562,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>208</v>
@@ -5622,7 +5622,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>213</v>
@@ -5678,7 +5678,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>156</v>
@@ -5738,7 +5738,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>167</v>
@@ -5798,7 +5798,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>175</v>
@@ -5858,7 +5858,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>180</v>
@@ -5918,7 +5918,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>186</v>
@@ -5972,7 +5972,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>218</v>
@@ -6034,7 +6034,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>225</v>
@@ -6094,7 +6094,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>230</v>
@@ -6152,7 +6152,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>236</v>
@@ -6212,7 +6212,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>244</v>
@@ -6270,7 +6270,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>252</v>
@@ -6330,7 +6330,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>259</v>
@@ -6388,7 +6388,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>265</v>
@@ -6448,7 +6448,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>271</v>
@@ -6508,7 +6508,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>277</v>
@@ -6568,7 +6568,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>284</v>
@@ -6626,7 +6626,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>292</v>
@@ -6684,7 +6684,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>297</v>
@@ -6742,7 +6742,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>302</v>
@@ -6802,7 +6802,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>309</v>
@@ -6854,7 +6854,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>315</v>
@@ -6910,7 +6910,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>321</v>
@@ -6972,7 +6972,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>327</v>
@@ -7030,7 +7030,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>332</v>
@@ -7088,7 +7088,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>335</v>
@@ -7150,7 +7150,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C71" s="6" t="s">
         <v>341</v>
@@ -7206,7 +7206,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>349</v>
@@ -7264,7 +7264,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>354</v>
@@ -7322,7 +7322,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C74" s="6" t="s">
         <v>360</v>
@@ -7380,7 +7380,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>367</v>
@@ -7442,7 +7442,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>373</v>
@@ -7496,7 +7496,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>378</v>
@@ -7556,7 +7556,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>382</v>
@@ -7612,7 +7612,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>388</v>
@@ -7668,7 +7668,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>393</v>
@@ -7726,7 +7726,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>400</v>
@@ -7782,7 +7782,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>407</v>
@@ -7842,7 +7842,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>414</v>
@@ -7900,7 +7900,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>421</v>
@@ -7960,7 +7960,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>426</v>
@@ -8020,7 +8020,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>431</v>
@@ -8074,7 +8074,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>437</v>
@@ -8128,7 +8128,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>444</v>
@@ -8182,7 +8182,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C89" s="3" t="s">
         <v>448</v>
@@ -8240,7 +8240,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C90" s="3" t="s">
         <v>455</v>
@@ -8296,7 +8296,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C91" s="3" t="s">
         <v>462</v>
@@ -8352,7 +8352,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C92" s="3" t="s">
         <v>467</v>
@@ -8410,7 +8410,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>475</v>
@@ -8464,7 +8464,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C94" s="3" t="s">
         <v>480</v>
@@ -8522,7 +8522,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C95" s="3" t="s">
         <v>488</v>
@@ -8574,7 +8574,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C96" s="3" t="s">
         <v>733</v>
@@ -8626,7 +8626,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>504</v>
@@ -8676,7 +8676,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C98" s="3" t="s">
         <v>508</v>
@@ -8728,7 +8728,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>734</v>
@@ -8780,7 +8780,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C100" s="3" t="s">
         <v>512</v>
@@ -8830,7 +8830,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C101" s="3" t="s">
         <v>515</v>
@@ -8880,7 +8880,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C102" s="3" t="s">
         <v>738</v>
@@ -8930,7 +8930,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C103" s="3" t="s">
         <v>520</v>
@@ -8980,7 +8980,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>524</v>
@@ -9030,7 +9030,7 @@
         <v>104</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>527</v>
@@ -9082,7 +9082,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>533</v>
@@ -9132,7 +9132,7 @@
         <v>106</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C107" s="3" t="s">
         <v>537</v>
@@ -9184,7 +9184,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C108" s="3" t="s">
         <v>544</v>
@@ -9233,7 +9233,7 @@
         <v>108</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C109" s="3" t="s">
         <v>552</v>
@@ -9282,7 +9282,7 @@
         <v>109</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C110" s="3" t="s">
         <v>565</v>
@@ -9334,7 +9334,7 @@
         <v>110</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C111" s="3" t="s">
         <v>741</v>
@@ -9386,7 +9386,7 @@
         <v>111</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C112" s="3" t="s">
         <v>564</v>
@@ -9438,7 +9438,7 @@
         <v>112</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C113" s="3" t="s">
         <v>571</v>
@@ -9490,7 +9490,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C114" s="3" t="s">
         <v>752</v>
@@ -9538,7 +9538,7 @@
         <v>114</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C115" s="3" t="s">
         <v>757</v>
@@ -9584,7 +9584,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C116" s="3" t="s">
         <v>760</v>
@@ -9632,7 +9632,7 @@
         <v>116</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C117" s="3" t="s">
         <v>765</v>
@@ -9678,7 +9678,7 @@
         <v>117</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C118" s="3" t="s">
         <v>769</v>
@@ -9724,7 +9724,7 @@
         <v>118</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C119" s="3" t="s">
         <v>577</v>
@@ -9772,7 +9772,7 @@
         <v>119</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C120" s="3" t="s">
         <v>583</v>
@@ -9820,7 +9820,7 @@
         <v>120</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C121" s="3" t="s">
         <v>588</v>
@@ -9870,7 +9870,7 @@
         <v>121</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C122" s="3" t="s">
         <v>594</v>
@@ -9916,7 +9916,7 @@
         <v>122</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C123" s="3" t="s">
         <v>746</v>
@@ -9962,7 +9962,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C124" s="3" t="s">
         <v>599</v>
@@ -10006,7 +10006,7 @@
         <v>124</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C125" s="3" t="s">
         <v>604</v>
@@ -10054,7 +10054,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C126" s="3" t="s">
         <v>609</v>
@@ -10102,7 +10102,7 @@
         <v>126</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C127" s="3" t="s">
         <v>615</v>
@@ -10152,7 +10152,7 @@
         <v>127</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C128" s="3" t="s">
         <v>620</v>
@@ -10200,7 +10200,7 @@
         <v>128</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C129" s="3" t="s">
         <v>625</v>
@@ -10250,7 +10250,7 @@
         <v>129</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C130" s="3" t="s">
         <v>631</v>
@@ -10300,7 +10300,7 @@
         <v>130</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C131" s="3" t="s">
         <v>636</v>
@@ -10348,7 +10348,7 @@
         <v>131</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C132" s="3" t="s">
         <v>641</v>
@@ -10396,7 +10396,7 @@
         <v>132</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C133" s="3" t="s">
         <v>646</v>
@@ -10444,7 +10444,7 @@
         <v>133</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C134" s="3" t="s">
         <v>650</v>
@@ -10490,7 +10490,7 @@
         <v>134</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C135" t="s">
         <v>655</v>
@@ -10533,7 +10533,7 @@
         <v>135</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C136" s="3" t="s">
         <v>662</v>
@@ -10576,7 +10576,7 @@
         <v>136</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C137" s="3" t="s">
         <v>680</v>
@@ -10619,7 +10619,7 @@
         <v>137</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C138" s="3" t="s">
         <v>687</v>
@@ -10662,7 +10662,7 @@
         <v>138</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C139" s="3" t="s">
         <v>692</v>

</xml_diff>